<commit_message>
aaa	aaaa	aarti.kulkarni1	aarti.k	aarti.kulkarni1	Engineering	aartikulkarni25@yahoo.com	9503504845 aaa	aaaa	aarti.kulkarni1	aarti.k	aarti.kulkarni1	Engineering	aartikulkarni25@yahoo.com	9503504845
</commit_message>
<xml_diff>
--- a/src/main/java/DeltaxRegistration/Delatx_registartiongForm/data/deltax_data.xlsx
+++ b/src/main/java/DeltaxRegistration/Delatx_registartiongForm/data/deltax_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24030" windowHeight="10005"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14895" windowHeight="8325"/>
   </bookViews>
   <sheets>
     <sheet name="Register_data" sheetId="1" r:id="rId1"/>
@@ -16,9 +16,10 @@
     <sheet name="SpecialCharacters" sheetId="9" r:id="rId7"/>
     <sheet name="InvalidPassword" sheetId="6" r:id="rId8"/>
     <sheet name="InvalidconfirmPassword" sheetId="7" r:id="rId9"/>
+    <sheet name="InValidEmailAddresss" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="E1:T31"/>
+  <oleSize ref="E1:K25"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="29">
   <si>
     <t>FirstName</t>
   </si>
@@ -91,6 +92,30 @@
   </si>
   <si>
     <t>aarti</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>************</t>
+  </si>
+  <si>
+    <t>Pass@1234</t>
+  </si>
+  <si>
+    <t>aarti kulkarni1</t>
+  </si>
+  <si>
+    <t>kulkarni</t>
+  </si>
+  <si>
+    <t>Pass@      1234</t>
+  </si>
+  <si>
+    <t>aartikulkarni25</t>
+  </si>
+  <si>
+    <t>aartikulkarni25@yahoo</t>
   </si>
 </sst>
 </file>
@@ -424,7 +449,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,38 +517,120 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="3">
-        <v>9503504845</v>
-      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="7" max="7" width="43.5703125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="3">
+        <v>9503504845</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="3">
+        <v>9503504845</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="aartikulkarni25@yahoo.com"/>
     <hyperlink ref="G3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -746,7 +853,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H3"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,27 +1062,331 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="44" customWidth="1"/>
+    <col min="6" max="6" width="52" customWidth="1"/>
+    <col min="7" max="7" width="54.5703125" customWidth="1"/>
+    <col min="8" max="8" width="42.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3">
+        <v>9503504845</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3">
+        <v>9503504845</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="8" max="8" width="41.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3">
+        <v>9503504845</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3">
+        <v>9503504845</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3">
+        <v>9503504845</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="3">
+        <v>9503504845</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3">
+        <v>9503504845</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId5"/>
+    <hyperlink ref="D3" r:id="rId6"/>
+    <hyperlink ref="D6" r:id="rId7"/>
+    <hyperlink ref="D5" r:id="rId8"/>
+    <hyperlink ref="D7" r:id="rId9"/>
+    <hyperlink ref="G6" r:id="rId10"/>
+    <hyperlink ref="G7" r:id="rId11"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -984,14 +1395,17 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="36.28515625" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1"/>
+    <col min="8" max="8" width="57.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1086,11 +1500,13 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1"/>
     <col min="5" max="5" width="33.140625" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" customWidth="1"/>

</xml_diff>